<commit_message>
actualizacion del 3 de marzo pero solo algunos
</commit_message>
<xml_diff>
--- a/xlsx/a69_f02_bUPPachuca.xlsx
+++ b/xlsx/a69_f02_bUPPachuca.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3er Trimestre 2022\Recepción de Información\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432BAA0A-3111-499E-9789-CC11AD72FFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="615" windowWidth="13815" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -112,16 +106,16 @@
     <t>Nota</t>
   </si>
   <si>
-    <t>http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Abril-Junio/02_b/ESTRUCTURA%20ORGANICA%20%282%29.pdf</t>
-  </si>
-  <si>
     <t>Departamento de Recursos Humanos (UPP)</t>
+  </si>
+  <si>
+    <t>http://UPPachuca@transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Octubre-Diciembre/2b/CISCMRDE-003-2023%20UPP%20EO.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -194,14 +188,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -220,18 +212,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -266,39 +256,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,7 +323,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,151 +367,175 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,11 +543,11 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.28515625" customWidth="1"/>
+    <col min="4" max="4" width="92.28515625" customWidth="1"/>
     <col min="5" max="5" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -558,7 +572,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -665,29 +679,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2022</v>
       </c>
       <c r="B8" s="3">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C8" s="3">
-        <v>44834</v>
+        <v>44926</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" s="3">
-        <v>44844</v>
+        <v>44936</v>
       </c>
       <c r="G8" s="3">
-        <v>44844</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>44936</v>
+      </c>
+      <c r="H8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -700,9 +714,8 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" display="http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Abril-Junio/02_b/ESTRUCTURA ORGANICA %282%29.pdf" xr:uid="{4583CC32-FFA4-4BE2-A475-F0B4C2A92CE0}"/>
+    <hyperlink ref="D8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios maydeli antes de vacacioens
</commit_message>
<xml_diff>
--- a/xlsx/a69_f02_bUPPachuca.xlsx
+++ b/xlsx/a69_f02_bUPPachuca.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2023\SIPOT\1er Trimestre 2023\Recepción de Información\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\2023\SIPOT\2DO TRIMESTRE 2023\Pagina Oficial 2do Trimestre 2023\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D650ED9-AA4B-41AF-BDE8-D060A7515CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
+    <sheet name="Hidden_1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="Hidden_14">Hidden_1!$A$1:$A$2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>43965</t>
   </si>
@@ -51,6 +56,9 @@
     <t>7</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -72,6 +80,15 @@
     <t>345312</t>
   </si>
   <si>
+    <t>570755</t>
+  </si>
+  <si>
+    <t>570756</t>
+  </si>
+  <si>
+    <t>570757</t>
+  </si>
+  <si>
     <t>345313</t>
   </si>
   <si>
@@ -99,6 +116,15 @@
     <t>Hipervínculo al organigrama completo</t>
   </si>
   <si>
+    <t>ESTE CRITERIO APLICA A PARTIR DEL 01/07/2023 -&gt; ¿El sujeto obligado tiene entre sus atribuciones dar atención a temas relacionados con violencia y/o igualdad de género? (catálogo)</t>
+  </si>
+  <si>
+    <t>ESTE CRITERIO APLICA A PARTIR DEL 01/07/2023 -&gt; Denominación del área/s que, de conformidad con sus atribuciones, dan atención a temas relacionados con violencia y/o igualdad de género</t>
+  </si>
+  <si>
+    <t>ESTE CRITERIO APLICA A PARTIR DEL 01/07/2023 -&gt; En su caso, denominación del Comité o instancia que atiende temas de género, aun cuando no cuente con atribuciones expresas para ello</t>
+  </si>
+  <si>
     <t>Área(s) responsable(s) que genera(n), posee(n), publica(n) y actualizan la información</t>
   </si>
   <si>
@@ -111,16 +137,25 @@
     <t>Nota</t>
   </si>
   <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Departamento de Recursos Humanos (UPP)</t>
   </si>
   <si>
-    <t>http://UPPachuca@transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Octubre-Diciembre/2b/CISCMRDE-003-2023%20UPP%20EO.pdf</t>
+    <t>Unidad para la igualdad entre mujeres y hombres</t>
+  </si>
+  <si>
+    <t>https://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Octubre-Diciembre/2b/CISCMRDE-003-2023%20UPP%20EO.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,13 +169,11 @@
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -169,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -192,12 +225,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -208,16 +250,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -317,6 +358,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -352,6 +410,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -527,11 +602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,19 +614,22 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92.28515625" customWidth="1"/>
-    <col min="5" max="5" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="76.85546875" customWidth="1"/>
+    <col min="5" max="5" width="155.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="163" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="161.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -568,7 +646,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -579,13 +657,13 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -602,44 +680,62 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="46.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -648,60 +744,81 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2023</v>
       </c>
       <c r="B8" s="3">
-        <v>44927</v>
+        <v>45017</v>
       </c>
       <c r="C8" s="3">
-        <v>45016</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>45107</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="3">
-        <v>45026</v>
-      </c>
-      <c r="G8" s="3">
-        <v>45026</v>
-      </c>
-      <c r="H8" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45117</v>
+      </c>
+      <c r="J8" s="3">
+        <v>45117</v>
+      </c>
+      <c r="K8" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
@@ -709,9 +826,37 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E8:E201" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>Hidden_14</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{6EA308A0-CEC1-45A4-9600-BE3788C7DD2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>